<commit_message>
Finished adding data to rdeep and rand
</commit_message>
<xml_diff>
--- a/Text/research results.xlsx
+++ b/Text/research results.xlsx
@@ -97,7 +97,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -188,30 +187,30 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="V27" activeCellId="0" sqref="V27"/>
+      <selection pane="topRight" activeCell="S9" activeCellId="0" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.61224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.46938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.16836734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.18877551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.64285714285714"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.33163265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.52551020408163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.64285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="6.52551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -279,6 +278,60 @@
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -520,6 +573,60 @@
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B9" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -767,6 +874,24 @@
       <c r="M26" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="N26" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="P26" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="R26" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="S26" s="0" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -1043,6 +1168,24 @@
       </c>
       <c r="M31" s="0" t="n">
         <v>87</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added barplots for Rdeep,bully (incomplete) and rand. R source files present
</commit_message>
<xml_diff>
--- a/Text/research results.xlsx
+++ b/Text/research results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="26">
   <si>
     <t xml:space="preserve">Against Rand</t>
   </si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">ml</t>
   </si>
   <si>
-    <t xml:space="preserve">ml_advancedSImple</t>
+    <t xml:space="preserve">ml_enriched</t>
   </si>
   <si>
     <t xml:space="preserve">ml_advanced</t>
@@ -204,18 +204,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S69"/>
+  <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B91" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
-      <selection pane="topRight" activeCell="D121" activeCellId="0" sqref="D121"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B22" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topRight" activeCell="F52" activeCellId="0" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,65 +820,65 @@
       <c r="A31" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B31" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>98</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="H32" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>97</v>
-      </c>
-      <c r="K32" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="L32" s="0" t="n">
-        <v>79</v>
-      </c>
-      <c r="M32" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="N32" s="0" t="n">
-        <v>103</v>
-      </c>
-      <c r="O32" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="P32" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="Q32" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="R32" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="S32" s="0" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -1134,36 +1134,36 @@
       <c r="B41" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="1" t="e">
+      <c r="C41" s="1" t="n">
         <f aca="false">AVERAGE(B31,D31,F31,H31,J31,L31,N31,P31,R31)</f>
-        <v>#DIV/0!</v>
+        <v>93.6666666666667</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="1" t="e">
+      <c r="E41" s="1" t="n">
         <f aca="false">C41/120</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F41" s="1" t="e">
+        <v>0.780555555555556</v>
+      </c>
+      <c r="F41" s="1" t="n">
         <f aca="false">E41*100</f>
-        <v>#DIV/0!</v>
+        <v>78.0555555555556</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="1" t="n">
+      <c r="C42" s="1" t="e">
         <f aca="false">AVERAGE(B32,D32,F32,H32,J32,L32,N32,P32,R32)</f>
-        <v>93.6666666666667</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="1" t="e">
         <f aca="false">C42/120</f>
-        <v>0.780555555555556</v>
-      </c>
-      <c r="F42" s="1" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F42" s="1" t="e">
         <f aca="false">E42*100</f>
-        <v>78.0555555555556</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1651,6 +1651,128 @@
       </c>
       <c r="S69" s="0" t="n">
         <v>59</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <f aca="false">AVERAGE(B64,D64,F64,H64,J64,L64,N64,P64,R64)</f>
+        <v>38.6666666666667</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1" t="n">
+        <f aca="false">C74/120</f>
+        <v>0.322222222222222</v>
+      </c>
+      <c r="F74" s="1" t="n">
+        <f aca="false">E74*100</f>
+        <v>32.2222222222222</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="1" t="n">
+        <f aca="false">AVERAGE(B65,D65,F65,H65,J65,L65,N65,P65,R65)</f>
+        <v>31.4444444444444</v>
+      </c>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1" t="n">
+        <f aca="false">C75/120</f>
+        <v>0.262037037037037</v>
+      </c>
+      <c r="F75" s="1" t="n">
+        <f aca="false">E75*100</f>
+        <v>26.2037037037037</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <f aca="false">AVERAGE(B66,D66,F66,H66,J66,L66,N66,P66,R66)</f>
+        <v>28.5555555555556</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1" t="n">
+        <f aca="false">C76/120</f>
+        <v>0.237962962962963</v>
+      </c>
+      <c r="F76" s="1" t="n">
+        <f aca="false">E76*100</f>
+        <v>23.7962962962963</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <f aca="false">AVERAGE(B67,D67,F67,H67,J67,L67,N67,P67,R67)</f>
+        <v>31.5555555555556</v>
+      </c>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1" t="n">
+        <f aca="false">C77/120</f>
+        <v>0.262962962962963</v>
+      </c>
+      <c r="F77" s="1" t="n">
+        <f aca="false">E77*100</f>
+        <v>26.2962962962963</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <f aca="false">AVERAGE(B68,D68,F68,H68,J68,L68,N68,P68,R68)</f>
+        <v>32.4444444444444</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1" t="n">
+        <f aca="false">C78/120</f>
+        <v>0.27037037037037</v>
+      </c>
+      <c r="F78" s="1" t="n">
+        <f aca="false">E78*100</f>
+        <v>27.037037037037</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <f aca="false">AVERAGE(B69,D69,F69,H69,J69,L69,N69,P69,R69)</f>
+        <v>30.4444444444444</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1" t="n">
+        <f aca="false">C79/120</f>
+        <v>0.253703703703704</v>
+      </c>
+      <c r="F79" s="1" t="n">
+        <f aca="false">E79*100</f>
+        <v>25.3703703703704</v>
       </c>
     </row>
   </sheetData>
@@ -1674,30 +1796,30 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="S31" activeCellId="0" sqref="S31"/>
+      <selection pane="topRight" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,68 +2298,68 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>98</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>97</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>79</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>103</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="P16" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="Q16" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="R16" s="0" t="n">
-        <v>96</v>
-      </c>
-      <c r="S16" s="0" t="n">
-        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>